<commit_message>
map view 수정 완
</commit_message>
<xml_diff>
--- a/축제정보.xlsx
+++ b/축제정보.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\lsbigdata-gen4\project\3\3조_프로젝트_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\test-project\dashboard3\Yeongcheon_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -102,18 +102,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>영천</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>임실</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고흥</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>옥정호 벚꽃축제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -126,10 +114,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>문경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>전북 임실군 운암면 입석리 458</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -139,6 +123,22 @@
   </si>
   <si>
     <t>경북 문경시 동로면 노은2길 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영천시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>임실군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고흥군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문경시</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -147,7 +147,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -192,7 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -522,7 +522,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1">
         <v>7</v>
@@ -552,7 +552,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1">
         <v>7</v>
@@ -582,7 +582,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1">
         <v>7</v>
@@ -612,7 +612,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -642,7 +642,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -669,10 +669,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -688,7 +688,7 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H7" s="2">
         <v>35.633299999999998</v>
@@ -699,10 +699,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1">
         <v>4</v>
@@ -718,7 +718,7 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H8" s="2">
         <v>34.453499999999998</v>
@@ -729,10 +729,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -748,7 +748,7 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H9" s="2">
         <v>36.771500000000003</v>

</xml_diff>